<commit_message>
add import fe for returned products with Excel template
</commit_message>
<xml_diff>
--- a/public/assets/excel-templates/imports/aftersales/returned-product-import.xlsx
+++ b/public/assets/excel-templates/imports/aftersales/returned-product-import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\rekachain-web\public\assets\excel-templates\imports\aftersales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A53C52-3021-4D14-8128-1F4A12281017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75F56A4-2DEE-435E-8939-43843A707270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="2220" windowWidth="21600" windowHeight="11835" xr2:uid="{B7300B1D-39BB-45D7-99C0-682073213532}"/>
+    <workbookView xWindow="4785" yWindow="2565" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{B7300B1D-39BB-45D7-99C0-682073213532}"/>
   </bookViews>
   <sheets>
     <sheet name="Produk Retur" sheetId="1" r:id="rId1"/>
@@ -35,20 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Qty</t>
   </si>
   <si>
-    <t>Nomor Seri</t>
-  </si>
-  <si>
-    <t>Nama Produk</t>
-  </si>
-  <si>
-    <t>Tipe Produk</t>
-  </si>
-  <si>
     <t>Panel</t>
   </si>
   <si>
@@ -64,12 +55,6 @@
     <t>Panel Distribusi</t>
   </si>
   <si>
-    <t>Komponen Bermasalah</t>
-  </si>
-  <si>
-    <t>Penanganan</t>
-  </si>
-  <si>
     <t>Diganti</t>
   </si>
   <si>
@@ -82,21 +67,12 @@
     <t>Light</t>
   </si>
   <si>
-    <t>Seri Produk</t>
-  </si>
-  <si>
-    <t>Customer (Opsional)</t>
-  </si>
-  <si>
     <t>INKA</t>
   </si>
   <si>
     <t>PT XYZ</t>
   </si>
   <si>
-    <t>Keterangan</t>
-  </si>
-  <si>
     <t>Patah</t>
   </si>
   <si>
@@ -107,6 +83,27 @@
   </si>
   <si>
     <t>Kabel Panel Distribusi</t>
+  </si>
+  <si>
+    <t>Serial Number</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Product Type</t>
+  </si>
+  <si>
+    <t>Customer (Optional)</t>
+  </si>
+  <si>
+    <t>Problem Component Name</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -195,11 +192,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F492DBDB-7A24-4E92-82BD-C1CF5C545CD2}" name="Nomor Seri"/>
-    <tableColumn id="2" xr3:uid="{3E458159-F364-425D-AC5D-7FD0A56D745C}" name="Nama Produk"/>
-    <tableColumn id="3" xr3:uid="{1A219B18-F10B-4119-BEAE-5ECAEECD2FCC}" name="Tipe Produk"/>
+    <tableColumn id="1" xr3:uid="{F492DBDB-7A24-4E92-82BD-C1CF5C545CD2}" name="Serial Number"/>
+    <tableColumn id="2" xr3:uid="{3E458159-F364-425D-AC5D-7FD0A56D745C}" name="Product Name"/>
+    <tableColumn id="3" xr3:uid="{1A219B18-F10B-4119-BEAE-5ECAEECD2FCC}" name="Product Type"/>
     <tableColumn id="6" xr3:uid="{0A00380E-FFFD-4CC3-934A-EFFE56381012}" name="Qty"/>
-    <tableColumn id="5" xr3:uid="{3F83E40A-D01E-499D-A480-DB5AC5796DB1}" name="Customer (Opsional)"/>
+    <tableColumn id="5" xr3:uid="{3F83E40A-D01E-499D-A480-DB5AC5796DB1}" name="Customer (Optional)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -214,10 +211,10 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{18D610D8-81B3-4343-8B54-02F3A3EB617D}" name="Seri Produk"/>
-    <tableColumn id="2" xr3:uid="{B4B3E70E-BACA-47F7-9D7C-35164148A046}" name="Komponen Bermasalah"/>
-    <tableColumn id="4" xr3:uid="{AD9C62BB-634B-49EA-923D-302C8906A3D6}" name="Keterangan"/>
-    <tableColumn id="3" xr3:uid="{2DA4E1DE-BBC8-4C19-8C43-2AB785A23093}" name="Penanganan"/>
+    <tableColumn id="1" xr3:uid="{18D610D8-81B3-4343-8B54-02F3A3EB617D}" name="Serial Number"/>
+    <tableColumn id="2" xr3:uid="{B4B3E70E-BACA-47F7-9D7C-35164148A046}" name="Problem Component Name"/>
+    <tableColumn id="4" xr3:uid="{AD9C62BB-634B-49EA-923D-302C8906A3D6}" name="Note"/>
+    <tableColumn id="3" xr3:uid="{2DA4E1DE-BBC8-4C19-8C43-2AB785A23093}" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -523,8 +520,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,19 +535,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -558,16 +555,16 @@
         <v>22580000001</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -575,16 +572,16 @@
         <v>22580000002</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -592,16 +589,16 @@
         <v>22580000003</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -625,29 +622,29 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -655,13 +652,13 @@
         <v>22580000001</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -669,13 +666,13 @@
         <v>22580000001</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -683,13 +680,13 @@
         <v>22580000002</v>
       </c>
       <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -697,13 +694,13 @@
         <v>22580000003</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add notes creation for product problems and returned products during import
</commit_message>
<xml_diff>
--- a/public/assets/excel-templates/imports/aftersales/returned-product-import.xlsx
+++ b/public/assets/excel-templates/imports/aftersales/returned-product-import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\rekachain-web\public\assets\excel-templates\imports\aftersales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75F56A4-2DEE-435E-8939-43843A707270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BA1F89-2488-4FBF-A67A-D9BA4E19560B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="2565" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{B7300B1D-39BB-45D7-99C0-682073213532}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B7300B1D-39BB-45D7-99C0-682073213532}"/>
   </bookViews>
   <sheets>
     <sheet name="Produk Retur" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
-  <si>
-    <t>Qty</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Panel</t>
   </si>
@@ -104,6 +101,12 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Tidak Dingin</t>
+  </si>
+  <si>
+    <t>Tidak Berfungsi</t>
   </si>
 </sst>
 </file>
@@ -195,7 +198,7 @@
     <tableColumn id="1" xr3:uid="{F492DBDB-7A24-4E92-82BD-C1CF5C545CD2}" name="Serial Number"/>
     <tableColumn id="2" xr3:uid="{3E458159-F364-425D-AC5D-7FD0A56D745C}" name="Product Name"/>
     <tableColumn id="3" xr3:uid="{1A219B18-F10B-4119-BEAE-5ECAEECD2FCC}" name="Product Type"/>
-    <tableColumn id="6" xr3:uid="{0A00380E-FFFD-4CC3-934A-EFFE56381012}" name="Qty"/>
+    <tableColumn id="6" xr3:uid="{0A00380E-FFFD-4CC3-934A-EFFE56381012}" name="Note"/>
     <tableColumn id="5" xr3:uid="{3F83E40A-D01E-499D-A480-DB5AC5796DB1}" name="Customer (Optional)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -520,34 +523,34 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -555,16 +558,16 @@
         <v>22580000001</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -572,16 +575,16 @@
         <v>22580000002</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -589,16 +592,16 @@
         <v>22580000003</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -622,7 +625,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -635,16 +638,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -652,13 +655,13 @@
         <v>22580000001</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -666,13 +669,13 @@
         <v>22580000001</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,13 +683,13 @@
         <v>22580000002</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -694,13 +697,13 @@
         <v>22580000003</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>